<commit_message>
Been working in the park, nearly got things ready
</commit_message>
<xml_diff>
--- a/Flare Notes.xlsx
+++ b/Flare Notes.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10313"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E165526-2A31-DB48-B19F-75DFEC65FFCA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F11A4D9D-0894-3C42-BDB8-6D5A69F4F325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="40960" windowHeight="25140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="New Board" sheetId="11" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1895" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1896" uniqueCount="89">
   <si>
     <t>o</t>
   </si>
@@ -297,6 +297,9 @@
   </si>
   <si>
     <t>LEDs</t>
+  </si>
+  <si>
+    <t>maybe this line is intact</t>
   </si>
 </sst>
 </file>
@@ -1587,6 +1590,9 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1604,9 +1610,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -7530,7 +7533,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AA27" sqref="AA27"/>
+      <selection pane="bottomRight" activeCell="AF25" sqref="AF25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7752,19 +7755,19 @@
       <c r="AH3" s="13"/>
       <c r="AI3" s="13"/>
       <c r="AJ3" s="13"/>
-      <c r="AK3" s="230" t="s">
+      <c r="AK3" s="231" t="s">
         <v>79</v>
       </c>
-      <c r="AL3" s="230"/>
-      <c r="AM3" s="230"/>
-      <c r="AN3" s="230"/>
-      <c r="AO3" s="230"/>
-      <c r="AP3" s="230"/>
-      <c r="AQ3" s="230"/>
-      <c r="AR3" s="230"/>
-      <c r="AS3" s="230"/>
-      <c r="AT3" s="230"/>
-      <c r="AU3" s="230"/>
+      <c r="AL3" s="231"/>
+      <c r="AM3" s="231"/>
+      <c r="AN3" s="231"/>
+      <c r="AO3" s="231"/>
+      <c r="AP3" s="231"/>
+      <c r="AQ3" s="231"/>
+      <c r="AR3" s="231"/>
+      <c r="AS3" s="231"/>
+      <c r="AT3" s="231"/>
+      <c r="AU3" s="231"/>
       <c r="AV3" s="13"/>
       <c r="AW3" s="13"/>
       <c r="AX3" s="13"/>
@@ -7808,17 +7811,17 @@
       <c r="AH4" s="13"/>
       <c r="AI4" s="13"/>
       <c r="AJ4" s="13"/>
-      <c r="AK4" s="230"/>
-      <c r="AL4" s="230"/>
-      <c r="AM4" s="230"/>
-      <c r="AN4" s="230"/>
-      <c r="AO4" s="230"/>
-      <c r="AP4" s="230"/>
-      <c r="AQ4" s="230"/>
-      <c r="AR4" s="230"/>
-      <c r="AS4" s="230"/>
-      <c r="AT4" s="230"/>
-      <c r="AU4" s="230"/>
+      <c r="AK4" s="231"/>
+      <c r="AL4" s="231"/>
+      <c r="AM4" s="231"/>
+      <c r="AN4" s="231"/>
+      <c r="AO4" s="231"/>
+      <c r="AP4" s="231"/>
+      <c r="AQ4" s="231"/>
+      <c r="AR4" s="231"/>
+      <c r="AS4" s="231"/>
+      <c r="AT4" s="231"/>
+      <c r="AU4" s="231"/>
       <c r="AV4" s="13"/>
       <c r="AW4" s="13"/>
       <c r="AX4" s="13"/>
@@ -7891,17 +7894,17 @@
       <c r="AH5" s="13"/>
       <c r="AI5" s="13"/>
       <c r="AJ5" s="13"/>
-      <c r="AK5" s="230"/>
-      <c r="AL5" s="230"/>
-      <c r="AM5" s="230"/>
-      <c r="AN5" s="230"/>
-      <c r="AO5" s="230"/>
-      <c r="AP5" s="230"/>
-      <c r="AQ5" s="230"/>
-      <c r="AR5" s="230"/>
-      <c r="AS5" s="230"/>
-      <c r="AT5" s="230"/>
-      <c r="AU5" s="230"/>
+      <c r="AK5" s="231"/>
+      <c r="AL5" s="231"/>
+      <c r="AM5" s="231"/>
+      <c r="AN5" s="231"/>
+      <c r="AO5" s="231"/>
+      <c r="AP5" s="231"/>
+      <c r="AQ5" s="231"/>
+      <c r="AR5" s="231"/>
+      <c r="AS5" s="231"/>
+      <c r="AT5" s="231"/>
+      <c r="AU5" s="231"/>
       <c r="AV5" s="13"/>
       <c r="AW5" s="13"/>
       <c r="AX5" s="13"/>
@@ -7944,17 +7947,17 @@
       <c r="AH6" s="13"/>
       <c r="AI6" s="13"/>
       <c r="AJ6" s="13"/>
-      <c r="AK6" s="230"/>
-      <c r="AL6" s="230"/>
-      <c r="AM6" s="230"/>
-      <c r="AN6" s="230"/>
-      <c r="AO6" s="230"/>
-      <c r="AP6" s="230"/>
-      <c r="AQ6" s="230"/>
-      <c r="AR6" s="230"/>
-      <c r="AS6" s="230"/>
-      <c r="AT6" s="230"/>
-      <c r="AU6" s="230"/>
+      <c r="AK6" s="231"/>
+      <c r="AL6" s="231"/>
+      <c r="AM6" s="231"/>
+      <c r="AN6" s="231"/>
+      <c r="AO6" s="231"/>
+      <c r="AP6" s="231"/>
+      <c r="AQ6" s="231"/>
+      <c r="AR6" s="231"/>
+      <c r="AS6" s="231"/>
+      <c r="AT6" s="231"/>
+      <c r="AU6" s="231"/>
       <c r="AV6" s="13"/>
       <c r="AW6" s="13"/>
       <c r="AX6" s="13"/>
@@ -8001,7 +8004,7 @@
       <c r="P7" s="86" t="s">
         <v>0</v>
       </c>
-      <c r="Q7" s="236" t="s">
+      <c r="Q7" s="230" t="s">
         <v>47</v>
       </c>
       <c r="R7" s="15" t="s">
@@ -8029,17 +8032,17 @@
       <c r="AH7" s="13"/>
       <c r="AI7" s="13"/>
       <c r="AJ7" s="13"/>
-      <c r="AK7" s="230"/>
-      <c r="AL7" s="230"/>
-      <c r="AM7" s="230"/>
-      <c r="AN7" s="230"/>
-      <c r="AO7" s="230"/>
-      <c r="AP7" s="230"/>
-      <c r="AQ7" s="230"/>
-      <c r="AR7" s="230"/>
-      <c r="AS7" s="230"/>
-      <c r="AT7" s="230"/>
-      <c r="AU7" s="230"/>
+      <c r="AK7" s="231"/>
+      <c r="AL7" s="231"/>
+      <c r="AM7" s="231"/>
+      <c r="AN7" s="231"/>
+      <c r="AO7" s="231"/>
+      <c r="AP7" s="231"/>
+      <c r="AQ7" s="231"/>
+      <c r="AR7" s="231"/>
+      <c r="AS7" s="231"/>
+      <c r="AT7" s="231"/>
+      <c r="AU7" s="231"/>
       <c r="AV7" s="13"/>
       <c r="AW7" s="13"/>
       <c r="AX7" s="13"/>
@@ -8082,17 +8085,17 @@
       <c r="AH8" s="13"/>
       <c r="AI8" s="13"/>
       <c r="AJ8" s="13"/>
-      <c r="AK8" s="230"/>
-      <c r="AL8" s="230"/>
-      <c r="AM8" s="230"/>
-      <c r="AN8" s="230"/>
-      <c r="AO8" s="230"/>
-      <c r="AP8" s="230"/>
-      <c r="AQ8" s="230"/>
-      <c r="AR8" s="230"/>
-      <c r="AS8" s="230"/>
-      <c r="AT8" s="230"/>
-      <c r="AU8" s="230"/>
+      <c r="AK8" s="231"/>
+      <c r="AL8" s="231"/>
+      <c r="AM8" s="231"/>
+      <c r="AN8" s="231"/>
+      <c r="AO8" s="231"/>
+      <c r="AP8" s="231"/>
+      <c r="AQ8" s="231"/>
+      <c r="AR8" s="231"/>
+      <c r="AS8" s="231"/>
+      <c r="AT8" s="231"/>
+      <c r="AU8" s="231"/>
       <c r="AV8" s="13"/>
       <c r="AW8" s="13"/>
       <c r="AX8" s="13"/>
@@ -8165,17 +8168,17 @@
       <c r="AH9" s="13"/>
       <c r="AI9" s="13"/>
       <c r="AJ9" s="13"/>
-      <c r="AK9" s="230"/>
-      <c r="AL9" s="230"/>
-      <c r="AM9" s="230"/>
-      <c r="AN9" s="230"/>
-      <c r="AO9" s="230"/>
-      <c r="AP9" s="230"/>
-      <c r="AQ9" s="230"/>
-      <c r="AR9" s="230"/>
-      <c r="AS9" s="230"/>
-      <c r="AT9" s="230"/>
-      <c r="AU9" s="230"/>
+      <c r="AK9" s="231"/>
+      <c r="AL9" s="231"/>
+      <c r="AM9" s="231"/>
+      <c r="AN9" s="231"/>
+      <c r="AO9" s="231"/>
+      <c r="AP9" s="231"/>
+      <c r="AQ9" s="231"/>
+      <c r="AR9" s="231"/>
+      <c r="AS9" s="231"/>
+      <c r="AT9" s="231"/>
+      <c r="AU9" s="231"/>
       <c r="AV9" s="13"/>
       <c r="AW9" s="13"/>
       <c r="AX9" s="13"/>
@@ -8210,17 +8213,17 @@
       <c r="AH10" s="13"/>
       <c r="AI10" s="13"/>
       <c r="AJ10" s="13"/>
-      <c r="AK10" s="230"/>
-      <c r="AL10" s="230"/>
-      <c r="AM10" s="230"/>
-      <c r="AN10" s="230"/>
-      <c r="AO10" s="230"/>
-      <c r="AP10" s="230"/>
-      <c r="AQ10" s="230"/>
-      <c r="AR10" s="230"/>
-      <c r="AS10" s="230"/>
-      <c r="AT10" s="230"/>
-      <c r="AU10" s="230"/>
+      <c r="AK10" s="231"/>
+      <c r="AL10" s="231"/>
+      <c r="AM10" s="231"/>
+      <c r="AN10" s="231"/>
+      <c r="AO10" s="231"/>
+      <c r="AP10" s="231"/>
+      <c r="AQ10" s="231"/>
+      <c r="AR10" s="231"/>
+      <c r="AS10" s="231"/>
+      <c r="AT10" s="231"/>
+      <c r="AU10" s="231"/>
       <c r="AV10" s="13"/>
       <c r="AW10" s="13"/>
       <c r="AX10" s="13"/>
@@ -8296,17 +8299,17 @@
       <c r="AH11" s="13"/>
       <c r="AI11" s="13"/>
       <c r="AJ11" s="13"/>
-      <c r="AK11" s="230"/>
-      <c r="AL11" s="230"/>
-      <c r="AM11" s="230"/>
-      <c r="AN11" s="230"/>
-      <c r="AO11" s="230"/>
-      <c r="AP11" s="230"/>
-      <c r="AQ11" s="230"/>
-      <c r="AR11" s="230"/>
-      <c r="AS11" s="230"/>
-      <c r="AT11" s="230"/>
-      <c r="AU11" s="230"/>
+      <c r="AK11" s="231"/>
+      <c r="AL11" s="231"/>
+      <c r="AM11" s="231"/>
+      <c r="AN11" s="231"/>
+      <c r="AO11" s="231"/>
+      <c r="AP11" s="231"/>
+      <c r="AQ11" s="231"/>
+      <c r="AR11" s="231"/>
+      <c r="AS11" s="231"/>
+      <c r="AT11" s="231"/>
+      <c r="AU11" s="231"/>
       <c r="AV11" s="13"/>
       <c r="AW11" s="13"/>
       <c r="AX11" s="13"/>
@@ -8347,17 +8350,17 @@
       <c r="AH12" s="13"/>
       <c r="AI12" s="13"/>
       <c r="AJ12" s="13"/>
-      <c r="AK12" s="230"/>
-      <c r="AL12" s="230"/>
-      <c r="AM12" s="230"/>
-      <c r="AN12" s="230"/>
-      <c r="AO12" s="230"/>
-      <c r="AP12" s="230"/>
-      <c r="AQ12" s="230"/>
-      <c r="AR12" s="230"/>
-      <c r="AS12" s="230"/>
-      <c r="AT12" s="230"/>
-      <c r="AU12" s="230"/>
+      <c r="AK12" s="231"/>
+      <c r="AL12" s="231"/>
+      <c r="AM12" s="231"/>
+      <c r="AN12" s="231"/>
+      <c r="AO12" s="231"/>
+      <c r="AP12" s="231"/>
+      <c r="AQ12" s="231"/>
+      <c r="AR12" s="231"/>
+      <c r="AS12" s="231"/>
+      <c r="AT12" s="231"/>
+      <c r="AU12" s="231"/>
       <c r="AV12" s="13"/>
       <c r="AW12" s="13"/>
       <c r="AX12" s="13"/>
@@ -8433,17 +8436,17 @@
       <c r="AH13" s="13"/>
       <c r="AI13" s="13"/>
       <c r="AJ13" s="13"/>
-      <c r="AK13" s="230"/>
-      <c r="AL13" s="230"/>
-      <c r="AM13" s="230"/>
-      <c r="AN13" s="230"/>
-      <c r="AO13" s="230"/>
-      <c r="AP13" s="230"/>
-      <c r="AQ13" s="230"/>
-      <c r="AR13" s="230"/>
-      <c r="AS13" s="230"/>
-      <c r="AT13" s="230"/>
-      <c r="AU13" s="230"/>
+      <c r="AK13" s="231"/>
+      <c r="AL13" s="231"/>
+      <c r="AM13" s="231"/>
+      <c r="AN13" s="231"/>
+      <c r="AO13" s="231"/>
+      <c r="AP13" s="231"/>
+      <c r="AQ13" s="231"/>
+      <c r="AR13" s="231"/>
+      <c r="AS13" s="231"/>
+      <c r="AT13" s="231"/>
+      <c r="AU13" s="231"/>
       <c r="AV13" s="13"/>
       <c r="AW13" s="13"/>
       <c r="AX13" s="13"/>
@@ -8484,17 +8487,17 @@
       <c r="AH14" s="13"/>
       <c r="AI14" s="13"/>
       <c r="AJ14" s="13"/>
-      <c r="AK14" s="230"/>
-      <c r="AL14" s="230"/>
-      <c r="AM14" s="230"/>
-      <c r="AN14" s="230"/>
-      <c r="AO14" s="230"/>
-      <c r="AP14" s="230"/>
-      <c r="AQ14" s="230"/>
-      <c r="AR14" s="230"/>
-      <c r="AS14" s="230"/>
-      <c r="AT14" s="230"/>
-      <c r="AU14" s="230"/>
+      <c r="AK14" s="231"/>
+      <c r="AL14" s="231"/>
+      <c r="AM14" s="231"/>
+      <c r="AN14" s="231"/>
+      <c r="AO14" s="231"/>
+      <c r="AP14" s="231"/>
+      <c r="AQ14" s="231"/>
+      <c r="AR14" s="231"/>
+      <c r="AS14" s="231"/>
+      <c r="AT14" s="231"/>
+      <c r="AU14" s="231"/>
       <c r="AV14" s="13"/>
       <c r="AW14" s="13"/>
       <c r="AX14" s="13"/>
@@ -8695,7 +8698,9 @@
       </c>
       <c r="U17" s="14"/>
       <c r="V17" s="186"/>
-      <c r="W17" s="186"/>
+      <c r="W17" s="193" t="s">
+        <v>88</v>
+      </c>
       <c r="X17" s="186"/>
       <c r="Y17" s="186"/>
       <c r="Z17" s="186"/>
@@ -8987,11 +8992,11 @@
       <c r="AH21" s="13"/>
       <c r="AI21" s="13"/>
       <c r="AJ21" s="13"/>
-      <c r="AK21" s="231">
+      <c r="AK21" s="232">
         <f>8.1*5</f>
         <v>40.5</v>
       </c>
-      <c r="AL21" s="231"/>
+      <c r="AL21" s="232"/>
       <c r="AM21" s="209" t="s">
         <v>83</v>
       </c>
@@ -9128,11 +9133,11 @@
       <c r="AH23" s="13"/>
       <c r="AI23" s="13"/>
       <c r="AJ23" s="13"/>
-      <c r="AK23" s="231">
+      <c r="AK23" s="232">
         <f>25</f>
         <v>25</v>
       </c>
-      <c r="AL23" s="231"/>
+      <c r="AL23" s="232"/>
       <c r="AM23" s="209" t="s">
         <v>84</v>
       </c>
@@ -12176,11 +12181,11 @@
       <c r="AT15" s="128" t="s">
         <v>0</v>
       </c>
-      <c r="AU15" s="232" t="s">
+      <c r="AU15" s="233" t="s">
         <v>60</v>
       </c>
-      <c r="AV15" s="232"/>
-      <c r="AW15" s="232"/>
+      <c r="AV15" s="233"/>
+      <c r="AW15" s="233"/>
       <c r="AX15" s="128" t="s">
         <v>0</v>
       </c>
@@ -16281,20 +16286,20 @@
       <c r="N54" s="30"/>
       <c r="O54" s="30"/>
       <c r="P54" s="30"/>
-      <c r="Q54" s="233" t="s">
+      <c r="Q54" s="234" t="s">
         <v>79</v>
       </c>
-      <c r="R54" s="234"/>
-      <c r="S54" s="234"/>
-      <c r="T54" s="234"/>
-      <c r="U54" s="234"/>
-      <c r="V54" s="234"/>
-      <c r="W54" s="234"/>
-      <c r="X54" s="234"/>
-      <c r="Y54" s="234"/>
-      <c r="Z54" s="234"/>
-      <c r="AA54" s="234"/>
-      <c r="AB54" s="234"/>
+      <c r="R54" s="235"/>
+      <c r="S54" s="235"/>
+      <c r="T54" s="235"/>
+      <c r="U54" s="235"/>
+      <c r="V54" s="235"/>
+      <c r="W54" s="235"/>
+      <c r="X54" s="235"/>
+      <c r="Y54" s="235"/>
+      <c r="Z54" s="235"/>
+      <c r="AA54" s="235"/>
+      <c r="AB54" s="235"/>
       <c r="AC54" s="30"/>
       <c r="AD54" s="30"/>
       <c r="AE54" s="30"/>
@@ -16334,18 +16339,18 @@
       <c r="N55" s="30"/>
       <c r="O55" s="30"/>
       <c r="P55" s="30"/>
-      <c r="Q55" s="234"/>
-      <c r="R55" s="234"/>
-      <c r="S55" s="234"/>
-      <c r="T55" s="234"/>
-      <c r="U55" s="234"/>
-      <c r="V55" s="234"/>
-      <c r="W55" s="234"/>
-      <c r="X55" s="234"/>
-      <c r="Y55" s="234"/>
-      <c r="Z55" s="234"/>
-      <c r="AA55" s="234"/>
-      <c r="AB55" s="234"/>
+      <c r="Q55" s="235"/>
+      <c r="R55" s="235"/>
+      <c r="S55" s="235"/>
+      <c r="T55" s="235"/>
+      <c r="U55" s="235"/>
+      <c r="V55" s="235"/>
+      <c r="W55" s="235"/>
+      <c r="X55" s="235"/>
+      <c r="Y55" s="235"/>
+      <c r="Z55" s="235"/>
+      <c r="AA55" s="235"/>
+      <c r="AB55" s="235"/>
       <c r="AC55" s="30"/>
       <c r="AD55" s="30"/>
       <c r="AE55" s="30"/>
@@ -16445,18 +16450,18 @@
       <c r="N56" s="1"/>
       <c r="O56" s="1"/>
       <c r="P56" s="1"/>
-      <c r="Q56" s="234"/>
-      <c r="R56" s="234"/>
-      <c r="S56" s="234"/>
-      <c r="T56" s="234"/>
-      <c r="U56" s="234"/>
-      <c r="V56" s="234"/>
-      <c r="W56" s="234"/>
-      <c r="X56" s="234"/>
-      <c r="Y56" s="234"/>
-      <c r="Z56" s="234"/>
-      <c r="AA56" s="234"/>
-      <c r="AB56" s="234"/>
+      <c r="Q56" s="235"/>
+      <c r="R56" s="235"/>
+      <c r="S56" s="235"/>
+      <c r="T56" s="235"/>
+      <c r="U56" s="235"/>
+      <c r="V56" s="235"/>
+      <c r="W56" s="235"/>
+      <c r="X56" s="235"/>
+      <c r="Y56" s="235"/>
+      <c r="Z56" s="235"/>
+      <c r="AA56" s="235"/>
+      <c r="AB56" s="235"/>
       <c r="AC56" s="1"/>
       <c r="AD56" s="1"/>
       <c r="AE56" s="1"/>
@@ -16512,18 +16517,18 @@
       <c r="N57" s="1"/>
       <c r="O57" s="1"/>
       <c r="P57" s="1"/>
-      <c r="Q57" s="234"/>
-      <c r="R57" s="234"/>
-      <c r="S57" s="234"/>
-      <c r="T57" s="234"/>
-      <c r="U57" s="234"/>
-      <c r="V57" s="234"/>
-      <c r="W57" s="234"/>
-      <c r="X57" s="234"/>
-      <c r="Y57" s="234"/>
-      <c r="Z57" s="234"/>
-      <c r="AA57" s="234"/>
-      <c r="AB57" s="234"/>
+      <c r="Q57" s="235"/>
+      <c r="R57" s="235"/>
+      <c r="S57" s="235"/>
+      <c r="T57" s="235"/>
+      <c r="U57" s="235"/>
+      <c r="V57" s="235"/>
+      <c r="W57" s="235"/>
+      <c r="X57" s="235"/>
+      <c r="Y57" s="235"/>
+      <c r="Z57" s="235"/>
+      <c r="AA57" s="235"/>
+      <c r="AB57" s="235"/>
       <c r="AC57" s="1"/>
       <c r="AD57" s="1"/>
       <c r="AE57" s="1"/>
@@ -16611,18 +16616,18 @@
       <c r="N58" s="30"/>
       <c r="O58" s="30"/>
       <c r="P58" s="30"/>
-      <c r="Q58" s="234"/>
-      <c r="R58" s="234"/>
-      <c r="S58" s="234"/>
-      <c r="T58" s="234"/>
-      <c r="U58" s="234"/>
-      <c r="V58" s="234"/>
-      <c r="W58" s="234"/>
-      <c r="X58" s="234"/>
-      <c r="Y58" s="234"/>
-      <c r="Z58" s="234"/>
-      <c r="AA58" s="234"/>
-      <c r="AB58" s="234"/>
+      <c r="Q58" s="235"/>
+      <c r="R58" s="235"/>
+      <c r="S58" s="235"/>
+      <c r="T58" s="235"/>
+      <c r="U58" s="235"/>
+      <c r="V58" s="235"/>
+      <c r="W58" s="235"/>
+      <c r="X58" s="235"/>
+      <c r="Y58" s="235"/>
+      <c r="Z58" s="235"/>
+      <c r="AA58" s="235"/>
+      <c r="AB58" s="235"/>
       <c r="AC58" s="30"/>
       <c r="AD58" s="30"/>
       <c r="AE58" s="30"/>
@@ -16669,18 +16674,18 @@
       <c r="N59" s="30"/>
       <c r="O59" s="30"/>
       <c r="P59" s="30"/>
-      <c r="Q59" s="234"/>
-      <c r="R59" s="234"/>
-      <c r="S59" s="234"/>
-      <c r="T59" s="234"/>
-      <c r="U59" s="234"/>
-      <c r="V59" s="234"/>
-      <c r="W59" s="234"/>
-      <c r="X59" s="234"/>
-      <c r="Y59" s="234"/>
-      <c r="Z59" s="234"/>
-      <c r="AA59" s="234"/>
-      <c r="AB59" s="234"/>
+      <c r="Q59" s="235"/>
+      <c r="R59" s="235"/>
+      <c r="S59" s="235"/>
+      <c r="T59" s="235"/>
+      <c r="U59" s="235"/>
+      <c r="V59" s="235"/>
+      <c r="W59" s="235"/>
+      <c r="X59" s="235"/>
+      <c r="Y59" s="235"/>
+      <c r="Z59" s="235"/>
+      <c r="AA59" s="235"/>
+      <c r="AB59" s="235"/>
       <c r="AC59" s="30"/>
       <c r="AD59" s="30"/>
       <c r="AE59" s="30"/>
@@ -16769,18 +16774,18 @@
       <c r="N60" s="30"/>
       <c r="O60" s="30"/>
       <c r="P60" s="30"/>
-      <c r="Q60" s="234"/>
-      <c r="R60" s="234"/>
-      <c r="S60" s="234"/>
-      <c r="T60" s="234"/>
-      <c r="U60" s="234"/>
-      <c r="V60" s="234"/>
-      <c r="W60" s="234"/>
-      <c r="X60" s="234"/>
-      <c r="Y60" s="234"/>
-      <c r="Z60" s="234"/>
-      <c r="AA60" s="234"/>
-      <c r="AB60" s="234"/>
+      <c r="Q60" s="235"/>
+      <c r="R60" s="235"/>
+      <c r="S60" s="235"/>
+      <c r="T60" s="235"/>
+      <c r="U60" s="235"/>
+      <c r="V60" s="235"/>
+      <c r="W60" s="235"/>
+      <c r="X60" s="235"/>
+      <c r="Y60" s="235"/>
+      <c r="Z60" s="235"/>
+      <c r="AA60" s="235"/>
+      <c r="AB60" s="235"/>
       <c r="AC60" s="30"/>
       <c r="AD60" s="30"/>
       <c r="AE60" s="30"/>
@@ -16827,18 +16832,18 @@
       <c r="N61" s="30"/>
       <c r="O61" s="30"/>
       <c r="P61" s="30"/>
-      <c r="Q61" s="234"/>
-      <c r="R61" s="234"/>
-      <c r="S61" s="234"/>
-      <c r="T61" s="234"/>
-      <c r="U61" s="234"/>
-      <c r="V61" s="234"/>
-      <c r="W61" s="234"/>
-      <c r="X61" s="234"/>
-      <c r="Y61" s="234"/>
-      <c r="Z61" s="234"/>
-      <c r="AA61" s="234"/>
-      <c r="AB61" s="234"/>
+      <c r="Q61" s="235"/>
+      <c r="R61" s="235"/>
+      <c r="S61" s="235"/>
+      <c r="T61" s="235"/>
+      <c r="U61" s="235"/>
+      <c r="V61" s="235"/>
+      <c r="W61" s="235"/>
+      <c r="X61" s="235"/>
+      <c r="Y61" s="235"/>
+      <c r="Z61" s="235"/>
+      <c r="AA61" s="235"/>
+      <c r="AB61" s="235"/>
       <c r="AC61" s="30"/>
       <c r="AD61" s="30"/>
       <c r="AE61" s="30"/>
@@ -16926,18 +16931,18 @@
       <c r="N62" s="30"/>
       <c r="O62" s="30"/>
       <c r="P62" s="30"/>
-      <c r="Q62" s="234"/>
-      <c r="R62" s="234"/>
-      <c r="S62" s="234"/>
-      <c r="T62" s="234"/>
-      <c r="U62" s="234"/>
-      <c r="V62" s="234"/>
-      <c r="W62" s="234"/>
-      <c r="X62" s="234"/>
-      <c r="Y62" s="234"/>
-      <c r="Z62" s="234"/>
-      <c r="AA62" s="234"/>
-      <c r="AB62" s="234"/>
+      <c r="Q62" s="235"/>
+      <c r="R62" s="235"/>
+      <c r="S62" s="235"/>
+      <c r="T62" s="235"/>
+      <c r="U62" s="235"/>
+      <c r="V62" s="235"/>
+      <c r="W62" s="235"/>
+      <c r="X62" s="235"/>
+      <c r="Y62" s="235"/>
+      <c r="Z62" s="235"/>
+      <c r="AA62" s="235"/>
+      <c r="AB62" s="235"/>
       <c r="AC62" s="30"/>
       <c r="AD62" s="30"/>
       <c r="AE62" s="30"/>
@@ -16977,18 +16982,18 @@
       <c r="N63" s="30"/>
       <c r="O63" s="30"/>
       <c r="P63" s="30"/>
-      <c r="Q63" s="234"/>
-      <c r="R63" s="234"/>
-      <c r="S63" s="234"/>
-      <c r="T63" s="234"/>
-      <c r="U63" s="234"/>
-      <c r="V63" s="234"/>
-      <c r="W63" s="234"/>
-      <c r="X63" s="234"/>
-      <c r="Y63" s="234"/>
-      <c r="Z63" s="234"/>
-      <c r="AA63" s="234"/>
-      <c r="AB63" s="234"/>
+      <c r="Q63" s="235"/>
+      <c r="R63" s="235"/>
+      <c r="S63" s="235"/>
+      <c r="T63" s="235"/>
+      <c r="U63" s="235"/>
+      <c r="V63" s="235"/>
+      <c r="W63" s="235"/>
+      <c r="X63" s="235"/>
+      <c r="Y63" s="235"/>
+      <c r="Z63" s="235"/>
+      <c r="AA63" s="235"/>
+      <c r="AB63" s="235"/>
       <c r="AC63" s="30"/>
       <c r="AD63" s="30"/>
       <c r="AE63" s="30"/>
@@ -17076,18 +17081,18 @@
       <c r="N64" s="30"/>
       <c r="O64" s="30"/>
       <c r="P64" s="30"/>
-      <c r="Q64" s="234"/>
-      <c r="R64" s="234"/>
-      <c r="S64" s="234"/>
-      <c r="T64" s="234"/>
-      <c r="U64" s="234"/>
-      <c r="V64" s="234"/>
-      <c r="W64" s="234"/>
-      <c r="X64" s="234"/>
-      <c r="Y64" s="234"/>
-      <c r="Z64" s="234"/>
-      <c r="AA64" s="234"/>
-      <c r="AB64" s="234"/>
+      <c r="Q64" s="235"/>
+      <c r="R64" s="235"/>
+      <c r="S64" s="235"/>
+      <c r="T64" s="235"/>
+      <c r="U64" s="235"/>
+      <c r="V64" s="235"/>
+      <c r="W64" s="235"/>
+      <c r="X64" s="235"/>
+      <c r="Y64" s="235"/>
+      <c r="Z64" s="235"/>
+      <c r="AA64" s="235"/>
+      <c r="AB64" s="235"/>
       <c r="AC64" s="30"/>
       <c r="AD64" s="30"/>
       <c r="AE64" s="30"/>
@@ -17127,18 +17132,18 @@
       <c r="N65" s="30"/>
       <c r="O65" s="30"/>
       <c r="P65" s="30"/>
-      <c r="Q65" s="234"/>
-      <c r="R65" s="234"/>
-      <c r="S65" s="234"/>
-      <c r="T65" s="234"/>
-      <c r="U65" s="234"/>
-      <c r="V65" s="234"/>
-      <c r="W65" s="234"/>
-      <c r="X65" s="234"/>
-      <c r="Y65" s="234"/>
-      <c r="Z65" s="234"/>
-      <c r="AA65" s="234"/>
-      <c r="AB65" s="234"/>
+      <c r="Q65" s="235"/>
+      <c r="R65" s="235"/>
+      <c r="S65" s="235"/>
+      <c r="T65" s="235"/>
+      <c r="U65" s="235"/>
+      <c r="V65" s="235"/>
+      <c r="W65" s="235"/>
+      <c r="X65" s="235"/>
+      <c r="Y65" s="235"/>
+      <c r="Z65" s="235"/>
+      <c r="AA65" s="235"/>
+      <c r="AB65" s="235"/>
       <c r="AC65" s="30"/>
       <c r="AD65" s="30"/>
       <c r="AE65" s="30"/>
@@ -17224,18 +17229,18 @@
       <c r="N66" s="30"/>
       <c r="O66" s="30"/>
       <c r="P66" s="30"/>
-      <c r="Q66" s="234"/>
-      <c r="R66" s="234"/>
-      <c r="S66" s="234"/>
-      <c r="T66" s="234"/>
-      <c r="U66" s="234"/>
-      <c r="V66" s="234"/>
-      <c r="W66" s="234"/>
-      <c r="X66" s="234"/>
-      <c r="Y66" s="234"/>
-      <c r="Z66" s="234"/>
-      <c r="AA66" s="234"/>
-      <c r="AB66" s="234"/>
+      <c r="Q66" s="235"/>
+      <c r="R66" s="235"/>
+      <c r="S66" s="235"/>
+      <c r="T66" s="235"/>
+      <c r="U66" s="235"/>
+      <c r="V66" s="235"/>
+      <c r="W66" s="235"/>
+      <c r="X66" s="235"/>
+      <c r="Y66" s="235"/>
+      <c r="Z66" s="235"/>
+      <c r="AA66" s="235"/>
+      <c r="AB66" s="235"/>
       <c r="AC66" s="30"/>
       <c r="AD66" s="30"/>
       <c r="AE66" s="30"/>
@@ -17275,18 +17280,18 @@
       <c r="N67" s="30"/>
       <c r="O67" s="30"/>
       <c r="P67" s="30"/>
-      <c r="Q67" s="234"/>
-      <c r="R67" s="234"/>
-      <c r="S67" s="234"/>
-      <c r="T67" s="234"/>
-      <c r="U67" s="234"/>
-      <c r="V67" s="234"/>
-      <c r="W67" s="234"/>
-      <c r="X67" s="234"/>
-      <c r="Y67" s="234"/>
-      <c r="Z67" s="234"/>
-      <c r="AA67" s="234"/>
-      <c r="AB67" s="234"/>
+      <c r="Q67" s="235"/>
+      <c r="R67" s="235"/>
+      <c r="S67" s="235"/>
+      <c r="T67" s="235"/>
+      <c r="U67" s="235"/>
+      <c r="V67" s="235"/>
+      <c r="W67" s="235"/>
+      <c r="X67" s="235"/>
+      <c r="Y67" s="235"/>
+      <c r="Z67" s="235"/>
+      <c r="AA67" s="235"/>
+      <c r="AB67" s="235"/>
       <c r="AC67" s="30"/>
       <c r="AD67" s="30"/>
       <c r="AE67" s="30"/>
@@ -17374,18 +17379,18 @@
       <c r="N68" s="30"/>
       <c r="O68" s="30"/>
       <c r="P68" s="30"/>
-      <c r="Q68" s="234"/>
-      <c r="R68" s="234"/>
-      <c r="S68" s="234"/>
-      <c r="T68" s="234"/>
-      <c r="U68" s="234"/>
-      <c r="V68" s="234"/>
-      <c r="W68" s="234"/>
-      <c r="X68" s="234"/>
-      <c r="Y68" s="234"/>
-      <c r="Z68" s="234"/>
-      <c r="AA68" s="234"/>
-      <c r="AB68" s="234"/>
+      <c r="Q68" s="235"/>
+      <c r="R68" s="235"/>
+      <c r="S68" s="235"/>
+      <c r="T68" s="235"/>
+      <c r="U68" s="235"/>
+      <c r="V68" s="235"/>
+      <c r="W68" s="235"/>
+      <c r="X68" s="235"/>
+      <c r="Y68" s="235"/>
+      <c r="Z68" s="235"/>
+      <c r="AA68" s="235"/>
+      <c r="AB68" s="235"/>
       <c r="AC68" s="30"/>
       <c r="AD68" s="30"/>
       <c r="AE68" s="30"/>
@@ -17425,18 +17430,18 @@
       <c r="N69" s="30"/>
       <c r="O69" s="30"/>
       <c r="P69" s="30"/>
-      <c r="Q69" s="234"/>
-      <c r="R69" s="234"/>
-      <c r="S69" s="234"/>
-      <c r="T69" s="234"/>
-      <c r="U69" s="234"/>
-      <c r="V69" s="234"/>
-      <c r="W69" s="234"/>
-      <c r="X69" s="234"/>
-      <c r="Y69" s="234"/>
-      <c r="Z69" s="234"/>
-      <c r="AA69" s="234"/>
-      <c r="AB69" s="234"/>
+      <c r="Q69" s="235"/>
+      <c r="R69" s="235"/>
+      <c r="S69" s="235"/>
+      <c r="T69" s="235"/>
+      <c r="U69" s="235"/>
+      <c r="V69" s="235"/>
+      <c r="W69" s="235"/>
+      <c r="X69" s="235"/>
+      <c r="Y69" s="235"/>
+      <c r="Z69" s="235"/>
+      <c r="AA69" s="235"/>
+      <c r="AB69" s="235"/>
       <c r="AC69" s="30"/>
       <c r="AD69" s="30"/>
       <c r="AE69" s="30"/>
@@ -17524,18 +17529,18 @@
       <c r="N70" s="30"/>
       <c r="O70" s="30"/>
       <c r="P70" s="30"/>
-      <c r="Q70" s="234"/>
-      <c r="R70" s="234"/>
-      <c r="S70" s="234"/>
-      <c r="T70" s="234"/>
-      <c r="U70" s="234"/>
-      <c r="V70" s="234"/>
-      <c r="W70" s="234"/>
-      <c r="X70" s="234"/>
-      <c r="Y70" s="234"/>
-      <c r="Z70" s="234"/>
-      <c r="AA70" s="234"/>
-      <c r="AB70" s="234"/>
+      <c r="Q70" s="235"/>
+      <c r="R70" s="235"/>
+      <c r="S70" s="235"/>
+      <c r="T70" s="235"/>
+      <c r="U70" s="235"/>
+      <c r="V70" s="235"/>
+      <c r="W70" s="235"/>
+      <c r="X70" s="235"/>
+      <c r="Y70" s="235"/>
+      <c r="Z70" s="235"/>
+      <c r="AA70" s="235"/>
+      <c r="AB70" s="235"/>
       <c r="AC70" s="30"/>
       <c r="AD70" s="30"/>
       <c r="AE70" s="30"/>
@@ -17571,18 +17576,18 @@
       <c r="BI70" s="122"/>
     </row>
     <row r="71" spans="13:61" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="Q71" s="234"/>
-      <c r="R71" s="234"/>
-      <c r="S71" s="234"/>
-      <c r="T71" s="234"/>
-      <c r="U71" s="234"/>
-      <c r="V71" s="234"/>
-      <c r="W71" s="234"/>
-      <c r="X71" s="234"/>
-      <c r="Y71" s="234"/>
-      <c r="Z71" s="234"/>
-      <c r="AA71" s="234"/>
-      <c r="AB71" s="234"/>
+      <c r="Q71" s="235"/>
+      <c r="R71" s="235"/>
+      <c r="S71" s="235"/>
+      <c r="T71" s="235"/>
+      <c r="U71" s="235"/>
+      <c r="V71" s="235"/>
+      <c r="W71" s="235"/>
+      <c r="X71" s="235"/>
+      <c r="Y71" s="235"/>
+      <c r="Z71" s="235"/>
+      <c r="AA71" s="235"/>
+      <c r="AB71" s="235"/>
       <c r="AL71" s="118" t="s">
         <v>0</v>
       </c>
@@ -17657,18 +17662,18 @@
       </c>
     </row>
     <row r="72" spans="13:61" x14ac:dyDescent="0.15">
-      <c r="Q72" s="234"/>
-      <c r="R72" s="234"/>
-      <c r="S72" s="234"/>
-      <c r="T72" s="234"/>
-      <c r="U72" s="234"/>
-      <c r="V72" s="234"/>
-      <c r="W72" s="234"/>
-      <c r="X72" s="234"/>
-      <c r="Y72" s="234"/>
-      <c r="Z72" s="234"/>
-      <c r="AA72" s="234"/>
-      <c r="AB72" s="234"/>
+      <c r="Q72" s="235"/>
+      <c r="R72" s="235"/>
+      <c r="S72" s="235"/>
+      <c r="T72" s="235"/>
+      <c r="U72" s="235"/>
+      <c r="V72" s="235"/>
+      <c r="W72" s="235"/>
+      <c r="X72" s="235"/>
+      <c r="Y72" s="235"/>
+      <c r="Z72" s="235"/>
+      <c r="AA72" s="235"/>
+      <c r="AB72" s="235"/>
       <c r="AL72" s="122"/>
       <c r="AM72" s="122"/>
       <c r="AN72" s="122"/>
@@ -17695,18 +17700,18 @@
       <c r="BI72" s="122"/>
     </row>
     <row r="73" spans="13:61" x14ac:dyDescent="0.15">
-      <c r="Q73" s="234"/>
-      <c r="R73" s="234"/>
-      <c r="S73" s="234"/>
-      <c r="T73" s="234"/>
-      <c r="U73" s="234"/>
-      <c r="V73" s="234"/>
-      <c r="W73" s="234"/>
-      <c r="X73" s="234"/>
-      <c r="Y73" s="234"/>
-      <c r="Z73" s="234"/>
-      <c r="AA73" s="234"/>
-      <c r="AB73" s="234"/>
+      <c r="Q73" s="235"/>
+      <c r="R73" s="235"/>
+      <c r="S73" s="235"/>
+      <c r="T73" s="235"/>
+      <c r="U73" s="235"/>
+      <c r="V73" s="235"/>
+      <c r="W73" s="235"/>
+      <c r="X73" s="235"/>
+      <c r="Y73" s="235"/>
+      <c r="Z73" s="235"/>
+      <c r="AA73" s="235"/>
+      <c r="AB73" s="235"/>
       <c r="AL73" s="118" t="s">
         <v>0</v>
       </c>
@@ -17781,18 +17786,18 @@
       </c>
     </row>
     <row r="74" spans="13:61" x14ac:dyDescent="0.15">
-      <c r="Q74" s="234"/>
-      <c r="R74" s="234"/>
-      <c r="S74" s="234"/>
-      <c r="T74" s="234"/>
-      <c r="U74" s="234"/>
-      <c r="V74" s="234"/>
-      <c r="W74" s="234"/>
-      <c r="X74" s="234"/>
-      <c r="Y74" s="234"/>
-      <c r="Z74" s="234"/>
-      <c r="AA74" s="234"/>
-      <c r="AB74" s="234"/>
+      <c r="Q74" s="235"/>
+      <c r="R74" s="235"/>
+      <c r="S74" s="235"/>
+      <c r="T74" s="235"/>
+      <c r="U74" s="235"/>
+      <c r="V74" s="235"/>
+      <c r="W74" s="235"/>
+      <c r="X74" s="235"/>
+      <c r="Y74" s="235"/>
+      <c r="Z74" s="235"/>
+      <c r="AA74" s="235"/>
+      <c r="AB74" s="235"/>
       <c r="AL74" s="122"/>
       <c r="AM74" s="122"/>
       <c r="AN74" s="122"/>
@@ -17819,18 +17824,18 @@
       <c r="BI74" s="122"/>
     </row>
     <row r="75" spans="13:61" x14ac:dyDescent="0.15">
-      <c r="Q75" s="234"/>
-      <c r="R75" s="234"/>
-      <c r="S75" s="234"/>
-      <c r="T75" s="234"/>
-      <c r="U75" s="234"/>
-      <c r="V75" s="234"/>
-      <c r="W75" s="234"/>
-      <c r="X75" s="234"/>
-      <c r="Y75" s="234"/>
-      <c r="Z75" s="234"/>
-      <c r="AA75" s="234"/>
-      <c r="AB75" s="234"/>
+      <c r="Q75" s="235"/>
+      <c r="R75" s="235"/>
+      <c r="S75" s="235"/>
+      <c r="T75" s="235"/>
+      <c r="U75" s="235"/>
+      <c r="V75" s="235"/>
+      <c r="W75" s="235"/>
+      <c r="X75" s="235"/>
+      <c r="Y75" s="235"/>
+      <c r="Z75" s="235"/>
+      <c r="AA75" s="235"/>
+      <c r="AB75" s="235"/>
       <c r="AL75" s="118" t="s">
         <v>0</v>
       </c>
@@ -17905,18 +17910,18 @@
       </c>
     </row>
     <row r="76" spans="13:61" ht="15" x14ac:dyDescent="0.15">
-      <c r="Q76" s="234"/>
-      <c r="R76" s="234"/>
-      <c r="S76" s="234"/>
-      <c r="T76" s="234"/>
-      <c r="U76" s="234"/>
-      <c r="V76" s="234"/>
-      <c r="W76" s="234"/>
-      <c r="X76" s="234"/>
-      <c r="Y76" s="234"/>
-      <c r="Z76" s="234"/>
-      <c r="AA76" s="234"/>
-      <c r="AB76" s="234"/>
+      <c r="Q76" s="235"/>
+      <c r="R76" s="235"/>
+      <c r="S76" s="235"/>
+      <c r="T76" s="235"/>
+      <c r="U76" s="235"/>
+      <c r="V76" s="235"/>
+      <c r="W76" s="235"/>
+      <c r="X76" s="235"/>
+      <c r="Y76" s="235"/>
+      <c r="Z76" s="235"/>
+      <c r="AA76" s="235"/>
+      <c r="AB76" s="235"/>
       <c r="AL76" s="126"/>
       <c r="AM76" s="126"/>
       <c r="AN76" s="126"/>
@@ -20591,26 +20596,26 @@
       <c r="N21" s="13"/>
       <c r="O21" s="13"/>
       <c r="P21" s="13"/>
-      <c r="Q21" s="235" t="s">
+      <c r="Q21" s="236" t="s">
         <v>35</v>
       </c>
-      <c r="R21" s="235"/>
-      <c r="S21" s="235"/>
-      <c r="T21" s="235"/>
-      <c r="U21" s="235"/>
-      <c r="V21" s="235"/>
-      <c r="W21" s="235"/>
-      <c r="X21" s="235"/>
-      <c r="Y21" s="235"/>
-      <c r="Z21" s="235"/>
-      <c r="AF21" s="235" t="s">
+      <c r="R21" s="236"/>
+      <c r="S21" s="236"/>
+      <c r="T21" s="236"/>
+      <c r="U21" s="236"/>
+      <c r="V21" s="236"/>
+      <c r="W21" s="236"/>
+      <c r="X21" s="236"/>
+      <c r="Y21" s="236"/>
+      <c r="Z21" s="236"/>
+      <c r="AF21" s="236" t="s">
         <v>36</v>
       </c>
-      <c r="AG21" s="235"/>
-      <c r="AH21" s="235"/>
-      <c r="AI21" s="235"/>
-      <c r="AJ21" s="235"/>
-      <c r="AK21" s="235"/>
+      <c r="AG21" s="236"/>
+      <c r="AH21" s="236"/>
+      <c r="AI21" s="236"/>
+      <c r="AJ21" s="236"/>
+      <c r="AK21" s="236"/>
     </row>
     <row r="22" spans="1:37" ht="5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
@@ -21327,14 +21332,14 @@
       <c r="Z37" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="AE37" s="235" t="s">
+      <c r="AE37" s="236" t="s">
         <v>37</v>
       </c>
-      <c r="AF37" s="235"/>
-      <c r="AG37" s="235"/>
-      <c r="AH37" s="235"/>
-      <c r="AI37" s="235"/>
-      <c r="AJ37" s="235"/>
+      <c r="AF37" s="236"/>
+      <c r="AG37" s="236"/>
+      <c r="AH37" s="236"/>
+      <c r="AI37" s="236"/>
+      <c r="AJ37" s="236"/>
     </row>
     <row r="38" spans="1:37" ht="5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>

</xml_diff>